<commit_message>
Updated the BOM to include categories and a pie chart. Waiting on links.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -36,6 +36,27 @@
   <si>
     <t>7 segment display</t>
   </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Hydrolics</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Raw Materials</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
 </sst>
 </file>
 
@@ -44,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +88,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -76,11 +105,293 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="21">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -90,10 +401,42 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -108,6 +451,159 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$3:$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Electronics</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hydrolics</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mechanical</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Raw Materials</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24.990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,159 +893,526 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F20"/>
+  <dimension ref="B1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="2"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="J2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="28">
+        <f>SUM(F4:F12)</f>
+        <v>24.990000000000002</v>
+      </c>
+      <c r="J3" s="8" t="str">
+        <f>B3</f>
+        <v>Electronics</v>
+      </c>
+      <c r="K3" s="23">
+        <f>G3</f>
+        <v>24.990000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="5">
         <v>10</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E4" s="6">
         <v>2.4990000000000001</v>
       </c>
-      <c r="F3" s="2">
-        <f>D3*E3</f>
+      <c r="F4" s="7">
+        <f>D4*E4</f>
         <v>24.990000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F4" s="2">
-        <f t="shared" ref="F4:F20" si="0">D4*E4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F5" s="2">
+      <c r="J4" s="8" t="str">
+        <f>B13</f>
+        <v>Hydrolics</v>
+      </c>
+      <c r="K4" s="23">
+        <f>G13</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="9">
+        <f t="shared" ref="F5:F21" si="0">D5*E5</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="8" t="str">
+        <f>B23</f>
+        <v>Mechanical</v>
+      </c>
+      <c r="K5" s="23">
+        <f>G23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="8"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F6" s="2">
+      <c r="J6" s="24" t="str">
+        <f>B33</f>
+        <v>Raw Materials</v>
+      </c>
+      <c r="K6" s="25">
+        <f>G33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="8"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F7" s="2">
+      <c r="J7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="27">
+        <f>SUM(K3:K6)</f>
+        <v>224.99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F8" s="2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F9" s="2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F10" s="2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="2">
-        <f t="shared" si="0"/>
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13">
+        <f>D12*E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="28">
+        <f>SUM(F14:F22)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6">
+        <v>100</v>
+      </c>
+      <c r="F14" s="7">
+        <f>D14*E14</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>100</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" ref="F15:F22" si="1">D15*E15</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13">
+        <f>D22*E22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="28">
+        <f>SUM(F24:F32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7">
+        <f>D24*E24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="9">
+        <f t="shared" ref="F25:F32" si="2">D25*E25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13">
+        <f>D32*E32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="28">
+        <f>SUM(F34:F42)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7">
+        <f>D34*E34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="9">
+        <f t="shared" ref="F35:F42" si="3">D35*E35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="8"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="8"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="8"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="10"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13">
+        <f>D42*E42</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B33:F33"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some stuff to the BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>Pump</t>
+  </si>
+  <si>
+    <t>Cylinder</t>
+  </si>
+  <si>
+    <t>http://www.grainger.com/product/MAXIM-Hydraulic-Cylinder-6FDA8?Pid=search</t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -421,6 +427,13 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -430,13 +443,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -530,7 +537,7 @@
                   <c:v>24.990000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>436.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -896,7 +903,7 @@
   <dimension ref="B1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,19 +933,19 @@
       <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="28">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="25">
         <f>SUM(F4:F12)</f>
         <v>24.990000000000002</v>
       </c>
@@ -946,7 +953,7 @@
         <f>B3</f>
         <v>Electronics</v>
       </c>
-      <c r="K3" s="23">
+      <c r="K3" s="20">
         <f>G3</f>
         <v>24.990000000000002</v>
       </c>
@@ -972,9 +979,9 @@
         <f>B13</f>
         <v>Hydrolics</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="20">
         <f>G13</f>
-        <v>200</v>
+        <v>436.5</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -983,14 +990,14 @@
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
       <c r="F5" s="9">
-        <f t="shared" ref="F5:F21" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F11" si="0">D5*E5</f>
         <v>0</v>
       </c>
       <c r="J5" s="8" t="str">
         <f>B23</f>
         <v>Mechanical</v>
       </c>
-      <c r="K5" s="23">
+      <c r="K5" s="20">
         <f>G23</f>
         <v>0</v>
       </c>
@@ -1004,11 +1011,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="24" t="str">
+      <c r="J6" s="21" t="str">
         <f>B33</f>
         <v>Raw Materials</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="22">
         <f>G33</f>
         <v>0</v>
       </c>
@@ -1022,12 +1029,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="24">
         <f>SUM(K3:K6)</f>
-        <v>224.99</v>
+        <v>461.49</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1081,16 +1088,16 @@
       </c>
     </row>
     <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="28">
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="25">
         <f>SUM(F14:F22)</f>
-        <v>200</v>
+        <v>436.5</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -1121,18 +1128,26 @@
         <v>100</v>
       </c>
       <c r="F15" s="9">
-        <f t="shared" ref="F15:F22" si="1">D15*E15</f>
+        <f t="shared" ref="F15:F21" si="1">D15*E15</f>
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
+      <c r="B16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>236.5</v>
+      </c>
       <c r="F16" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>236.5</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1196,14 +1211,14 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="28">
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="25">
         <f>SUM(F24:F32)</f>
         <v>0</v>
       </c>
@@ -1224,7 +1239,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="3"/>
       <c r="F25" s="9">
-        <f t="shared" ref="F25:F32" si="2">D25*E25</f>
+        <f t="shared" ref="F25:F31" si="2">D25*E25</f>
         <v>0</v>
       </c>
     </row>
@@ -1299,14 +1314,14 @@
       </c>
     </row>
     <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="28">
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="25">
         <f>SUM(F34:F42)</f>
         <v>0</v>
       </c>
@@ -1327,7 +1342,7 @@
       <c r="D35" s="2"/>
       <c r="E35" s="3"/>
       <c r="F35" s="9">
-        <f t="shared" ref="F35:F42" si="3">D35*E35</f>
+        <f t="shared" ref="F35:F41" si="3">D35*E35</f>
         <v>0</v>
       </c>
     </row>
@@ -1410,9 +1425,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C16" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>